<commit_message>
phase 1 time sereis pipelines added
</commit_message>
<xml_diff>
--- a/data/Lstm_Dates.xlsx
+++ b/data/Lstm_Dates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VenuraP\Desktop\Browns Data Projects\ML Projects\POC\Harti-Food-Price-Prediction\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF123C43-97BB-475C-A1A4-4B016E283C29}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C42ADE9-2B76-4705-8FEE-EF4647B30C6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -474,14 +474,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" customWidth="1"/>
+    <col min="1" max="1" width="20.21875" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
     <col min="4" max="4" width="18.21875" customWidth="1"/>
     <col min="5" max="5" width="18.44140625" customWidth="1"/>
     <col min="6" max="6" width="26.44140625" customWidth="1"/>

</xml_diff>